<commit_message>
Daily tasks solving additional
</commit_message>
<xml_diff>
--- a/Interview preposition 2019-2020.xlsx
+++ b/Interview preposition 2019-2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D791FE57-E7EA-4569-BC5E-8FA350CF512F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94E8B7E-BB3A-481D-A37D-400D772BDFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="297">
   <si>
     <t>Number</t>
   </si>
@@ -910,6 +910,9 @@
   </si>
   <si>
     <t>Binary Subarrays With Sum</t>
+  </si>
+  <si>
+    <t>Statistics from a Large Sample</t>
   </si>
 </sst>
 </file>
@@ -919,12 +922,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1089,7 +1100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1098,27 +1109,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1154,7 +1166,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C50ED8C-B740-45AF-BDA6-0857A5A322F4}" name="Таблица1" displayName="Таблица1" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{059DB994-AB16-4545-BFB1-8470F05D6AA7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G256">
+  <sortState ref="A2:G256">
     <sortCondition ref="G1:G1048576"/>
   </sortState>
   <tableColumns count="7">
@@ -1171,9 +1183,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1211,7 +1223,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1317,7 +1329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1468,24 +1480,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:G262"/>
+  <dimension ref="A1:G263"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="G261" sqref="G261"/>
+      <selection activeCell="G263" sqref="G263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>509</v>
       </c>
@@ -1531,7 +1543,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>766</v>
       </c>
@@ -1554,7 +1566,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>832</v>
       </c>
@@ -1577,7 +1589,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>867</v>
       </c>
@@ -1600,7 +1612,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>905</v>
       </c>
@@ -1623,7 +1635,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>922</v>
       </c>
@@ -1646,7 +1658,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>985</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>999</v>
       </c>
@@ -1692,7 +1704,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>1051</v>
       </c>
@@ -1715,7 +1727,7 @@
         <v>43642</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>238</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>43643</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>442</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>43643</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>950</v>
       </c>
@@ -1784,7 +1796,7 @@
         <v>43643</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>41</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>57</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>768</v>
       </c>
@@ -1853,7 +1865,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>769</v>
       </c>
@@ -1876,7 +1888,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>728</v>
       </c>
@@ -1899,7 +1911,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>812</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>868</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>883</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>908</v>
       </c>
@@ -1991,7 +2003,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>942</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1009</v>
       </c>
@@ -2037,7 +2049,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1103</v>
       </c>
@@ -2060,7 +2072,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>789</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>885</v>
       </c>
@@ -2106,7 +2118,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1006</v>
       </c>
@@ -2129,7 +2141,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1017</v>
       </c>
@@ -2152,7 +2164,7 @@
         <v>43648</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>335</v>
       </c>
@@ -2175,7 +2187,7 @@
         <v>43649</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>233</v>
       </c>
@@ -2198,7 +2210,7 @@
         <v>43651</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>780</v>
       </c>
@@ -2221,7 +2233,7 @@
         <v>43651</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>744</v>
       </c>
@@ -2244,7 +2256,7 @@
         <v>43652</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>43657</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>719</v>
       </c>
@@ -2290,7 +2302,7 @@
         <v>43657</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>657</v>
       </c>
@@ -2313,7 +2325,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>709</v>
       </c>
@@ -2336,7 +2348,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>804</v>
       </c>
@@ -2359,7 +2371,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>929</v>
       </c>
@@ -2382,7 +2394,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1108</v>
       </c>
@@ -2405,7 +2417,7 @@
         <v>43658</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>521</v>
       </c>
@@ -2428,7 +2440,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>824</v>
       </c>
@@ -2451,7 +2463,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>893</v>
       </c>
@@ -2474,7 +2486,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>917</v>
       </c>
@@ -2497,7 +2509,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>937</v>
       </c>
@@ -2520,7 +2532,7 @@
         <v>43659</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>890</v>
       </c>
@@ -2543,7 +2555,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>537</v>
       </c>
@@ -2566,7 +2578,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>791</v>
       </c>
@@ -2589,7 +2601,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1016</v>
       </c>
@@ -2612,7 +2624,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1106</v>
       </c>
@@ -2635,7 +2647,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>461</v>
       </c>
@@ -2658,7 +2670,7 @@
         <v>43667</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>476</v>
       </c>
@@ -2681,7 +2693,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>762</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>136</v>
       </c>
@@ -2727,7 +2739,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>190</v>
       </c>
@@ -2750,7 +2762,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>191</v>
       </c>
@@ -2773,7 +2785,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>231</v>
       </c>
@@ -2796,7 +2808,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>268</v>
       </c>
@@ -2819,7 +2831,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>342</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>371</v>
       </c>
@@ -2865,7 +2877,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>389</v>
       </c>
@@ -2888,7 +2900,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>405</v>
       </c>
@@ -2911,7 +2923,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>260</v>
       </c>
@@ -2934,7 +2946,7 @@
         <v>43670</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>137</v>
       </c>
@@ -2957,7 +2969,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>201</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>318</v>
       </c>
@@ -3003,7 +3015,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>477</v>
       </c>
@@ -3026,7 +3038,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>187</v>
       </c>
@@ -3049,7 +3061,7 @@
         <v>43672</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>88</v>
       </c>
@@ -3072,7 +3084,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>125</v>
       </c>
@@ -3095,7 +3107,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>345</v>
       </c>
@@ -3118,7 +3130,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>844</v>
       </c>
@@ -3141,7 +3153,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>925</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>977</v>
       </c>
@@ -3187,7 +3199,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>532</v>
       </c>
@@ -3210,7 +3222,7 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>11</v>
       </c>
@@ -3233,7 +3245,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>16</v>
       </c>
@@ -3256,7 +3268,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>986</v>
       </c>
@@ -3279,7 +3291,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>75</v>
       </c>
@@ -3302,7 +3314,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -3325,7 +3337,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A81" s="8">
         <v>904</v>
       </c>
@@ -3348,7 +3360,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>21</v>
       </c>
@@ -3371,7 +3383,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>237</v>
       </c>
@@ -3394,7 +3406,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>876</v>
       </c>
@@ -3417,7 +3429,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3440,7 +3452,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>203</v>
       </c>
@@ -3463,7 +3475,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>234</v>
       </c>
@@ -3486,7 +3498,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1019</v>
       </c>
@@ -3509,7 +3521,7 @@
         <v>43684</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>328</v>
       </c>
@@ -3555,7 +3567,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>445</v>
       </c>
@@ -3578,7 +3590,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>206</v>
       </c>
@@ -3601,7 +3613,7 @@
         <v>43687</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>725</v>
       </c>
@@ -3624,7 +3636,7 @@
         <v>43687</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>25</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>43689</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>92</v>
       </c>
@@ -3670,7 +3682,7 @@
         <v>43689</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>641</v>
       </c>
@@ -3693,7 +3705,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>622</v>
       </c>
@@ -3716,7 +3728,7 @@
         <v>43691</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>469</v>
       </c>
@@ -3739,7 +3751,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>682</v>
       </c>
@@ -3762,7 +3774,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>862</v>
       </c>
@@ -3785,7 +3797,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1047</v>
       </c>
@@ -3808,7 +3820,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>232</v>
       </c>
@@ -3831,7 +3843,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1021</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>20</v>
       </c>
@@ -3877,7 +3889,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>155</v>
       </c>
@@ -3900,7 +3912,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>225</v>
       </c>
@@ -3923,7 +3935,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>946</v>
       </c>
@@ -3946,7 +3958,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>503</v>
       </c>
@@ -3969,7 +3981,7 @@
         <v>43697</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>895</v>
       </c>
@@ -3992,7 +4004,7 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>50</v>
       </c>
@@ -4015,7 +4027,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>70</v>
       </c>
@@ -4038,7 +4050,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>95</v>
       </c>
@@ -4061,7 +4073,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>104</v>
       </c>
@@ -4084,7 +4096,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>118</v>
       </c>
@@ -4107,7 +4119,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>119</v>
       </c>
@@ -4130,7 +4142,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>775</v>
       </c>
@@ -4153,7 +4165,7 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>912</v>
       </c>
@@ -4176,7 +4188,7 @@
         <v>43707</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>98</v>
       </c>
@@ -4199,7 +4211,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>240</v>
       </c>
@@ -4222,7 +4234,7 @@
         <v>43710</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>37</v>
       </c>
@@ -4245,7 +4257,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>51</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>52</v>
       </c>
@@ -4291,7 +4303,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>17</v>
       </c>
@@ -4314,7 +4326,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>22</v>
       </c>
@@ -4337,7 +4349,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>46</v>
       </c>
@@ -4360,7 +4372,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>77</v>
       </c>
@@ -4383,7 +4395,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>100</v>
       </c>
@@ -4406,7 +4418,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>401</v>
       </c>
@@ -4429,7 +4441,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>784</v>
       </c>
@@ -4452,7 +4464,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>39</v>
       </c>
@@ -4475,7 +4487,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>40</v>
       </c>
@@ -4498,7 +4510,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>216</v>
       </c>
@@ -4521,7 +4533,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>1</v>
       </c>
@@ -4544,7 +4556,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>217</v>
       </c>
@@ -4567,7 +4579,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>219</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>349</v>
       </c>
@@ -4613,7 +4625,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>705</v>
       </c>
@@ -4636,7 +4648,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>706</v>
       </c>
@@ -4659,7 +4671,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>36</v>
       </c>
@@ -4682,7 +4694,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>49</v>
       </c>
@@ -4705,7 +4717,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>205</v>
       </c>
@@ -4728,7 +4740,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>387</v>
       </c>
@@ -4751,7 +4763,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>599</v>
       </c>
@@ -4774,7 +4786,7 @@
         <v>43720</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>3</v>
       </c>
@@ -4797,7 +4809,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>347</v>
       </c>
@@ -4820,7 +4832,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>380</v>
       </c>
@@ -4843,7 +4855,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>454</v>
       </c>
@@ -4866,7 +4878,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>652</v>
       </c>
@@ -4889,7 +4901,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>771</v>
       </c>
@@ -4912,7 +4924,7 @@
         <v>43721</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>144</v>
       </c>
@@ -4935,7 +4947,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>94</v>
       </c>
@@ -4958,7 +4970,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>102</v>
       </c>
@@ -4981,7 +4993,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>145</v>
       </c>
@@ -5004,7 +5016,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>101</v>
       </c>
@@ -5027,7 +5039,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>105</v>
       </c>
@@ -5050,7 +5062,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>106</v>
       </c>
@@ -5073,7 +5085,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>116</v>
       </c>
@@ -5096,7 +5108,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>117</v>
       </c>
@@ -5119,7 +5131,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>236</v>
       </c>
@@ -5142,7 +5154,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>297</v>
       </c>
@@ -5165,7 +5177,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>429</v>
       </c>
@@ -5188,7 +5200,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>559</v>
       </c>
@@ -5211,7 +5223,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>589</v>
       </c>
@@ -5234,7 +5246,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>590</v>
       </c>
@@ -5257,7 +5269,7 @@
         <v>43731</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>173</v>
       </c>
@@ -5280,7 +5292,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>700</v>
       </c>
@@ -5303,7 +5315,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>701</v>
       </c>
@@ -5326,7 +5338,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>450</v>
       </c>
@@ -5349,7 +5361,7 @@
         <v>43733</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>220</v>
       </c>
@@ -5372,7 +5384,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>108</v>
       </c>
@@ -5395,7 +5407,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>110</v>
       </c>
@@ -5418,7 +5430,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>208</v>
       </c>
@@ -5441,7 +5453,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>648</v>
       </c>
@@ -5464,7 +5476,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>677</v>
       </c>
@@ -5487,7 +5499,7 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>211</v>
       </c>
@@ -5510,7 +5522,7 @@
         <v>43751</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>421</v>
       </c>
@@ -5533,7 +5545,7 @@
         <v>43751</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>212</v>
       </c>
@@ -5556,7 +5568,7 @@
         <v>43752</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>336</v>
       </c>
@@ -5579,7 +5591,7 @@
         <v>43752</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>215</v>
       </c>
@@ -5602,7 +5614,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>378</v>
       </c>
@@ -5625,7 +5637,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>451</v>
       </c>
@@ -5648,7 +5660,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>973</v>
       </c>
@@ -5671,7 +5683,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>1046</v>
       </c>
@@ -5694,7 +5706,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>692</v>
       </c>
@@ -5717,7 +5729,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>720</v>
       </c>
@@ -5740,7 +5752,7 @@
         <v>43755</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>53</v>
       </c>
@@ -5763,7 +5775,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>121</v>
       </c>
@@ -5786,7 +5798,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>300</v>
       </c>
@@ -5809,7 +5821,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>1025</v>
       </c>
@@ -5832,7 +5844,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>1143</v>
       </c>
@@ -5855,7 +5867,7 @@
         <v>43763</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>72</v>
       </c>
@@ -5878,7 +5890,7 @@
         <v>43768</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>887</v>
       </c>
@@ -5901,7 +5913,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>91</v>
       </c>
@@ -5924,7 +5936,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>518</v>
       </c>
@@ -5947,7 +5959,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>1221</v>
       </c>
@@ -5970,7 +5982,7 @@
         <v>43773</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>944</v>
       </c>
@@ -5993,7 +6005,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>1029</v>
       </c>
@@ -6016,7 +6028,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>1217</v>
       </c>
@@ -6039,7 +6051,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>455</v>
       </c>
@@ -6062,7 +6074,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>860</v>
       </c>
@@ -6085,7 +6097,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>874</v>
       </c>
@@ -6108,7 +6120,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1005</v>
       </c>
@@ -6131,7 +6143,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>763</v>
       </c>
@@ -6154,7 +6166,7 @@
         <v>43776</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>921</v>
       </c>
@@ -6177,7 +6189,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>406</v>
       </c>
@@ -6200,7 +6212,7 @@
         <v>43778</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>1090</v>
       </c>
@@ -6223,7 +6235,7 @@
         <v>43778</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>765</v>
       </c>
@@ -6246,7 +6258,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>997</v>
       </c>
@@ -6269,7 +6281,7 @@
         <v>43782</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>1042</v>
       </c>
@@ -6292,7 +6304,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>1161</v>
       </c>
@@ -6315,7 +6327,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>841</v>
       </c>
@@ -6338,7 +6350,7 @@
         <v>43784</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>959</v>
       </c>
@@ -6361,7 +6373,7 @@
         <v>43784</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>1043</v>
       </c>
@@ -6384,7 +6396,7 @@
         <v>43784</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>399</v>
       </c>
@@ -6407,7 +6419,7 @@
         <v>43785</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>684</v>
       </c>
@@ -6430,7 +6442,7 @@
         <v>43785</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>802</v>
       </c>
@@ -6453,7 +6465,7 @@
         <v>43786</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>785</v>
       </c>
@@ -6476,7 +6488,7 @@
         <v>43787</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>996</v>
       </c>
@@ -6499,7 +6511,7 @@
         <v>43788</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>957</v>
       </c>
@@ -6522,7 +6534,7 @@
         <v>43789</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>938</v>
       </c>
@@ -6545,7 +6557,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>1266</v>
       </c>
@@ -6568,7 +6580,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>1281</v>
       </c>
@@ -6591,7 +6603,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>1290</v>
       </c>
@@ -6614,7 +6626,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>1295</v>
       </c>
@@ -6637,7 +6649,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>1313</v>
       </c>
@@ -6660,7 +6672,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>1323</v>
       </c>
@@ -6683,7 +6695,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>1252</v>
       </c>
@@ -6706,7 +6718,7 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>1309</v>
       </c>
@@ -6729,7 +6741,7 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>617</v>
       </c>
@@ -6752,7 +6764,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>961</v>
       </c>
@@ -6775,7 +6787,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>1299</v>
       </c>
@@ -6798,7 +6810,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>1304</v>
       </c>
@@ -6821,7 +6833,7 @@
         <v>43852</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>852</v>
       </c>
@@ -6844,7 +6856,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>965</v>
       </c>
@@ -6867,7 +6879,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>1122</v>
       </c>
@@ -6890,7 +6902,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>1207</v>
       </c>
@@ -6913,7 +6925,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>1237</v>
       </c>
@@ -6936,7 +6948,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>1329</v>
       </c>
@@ -6959,7 +6971,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>1331</v>
       </c>
@@ -6982,7 +6994,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>1332</v>
       </c>
@@ -7005,7 +7017,7 @@
         <v>43856</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>463</v>
       </c>
@@ -7028,7 +7040,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>884</v>
       </c>
@@ -7051,7 +7063,7 @@
         <v>43857</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>189</v>
       </c>
@@ -7074,7 +7086,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>897</v>
       </c>
@@ -7097,7 +7109,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>581</v>
       </c>
@@ -7120,7 +7132,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>665</v>
       </c>
@@ -7143,7 +7155,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>1222</v>
       </c>
@@ -7166,7 +7178,7 @@
         <v>43859</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>669</v>
       </c>
@@ -7189,7 +7201,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>1002</v>
       </c>
@@ -7212,7 +7224,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>1160</v>
       </c>
@@ -7235,7 +7247,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>1010</v>
       </c>
@@ -7258,7 +7270,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>821</v>
       </c>
@@ -7281,7 +7293,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>1200</v>
       </c>
@@ -7304,7 +7316,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>1341</v>
       </c>
@@ -7327,7 +7339,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>26</v>
       </c>
@@ -7350,7 +7362,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>27</v>
       </c>
@@ -7373,7 +7385,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>283</v>
       </c>
@@ -7396,7 +7408,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>1030</v>
       </c>
@@ -7419,7 +7431,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>872</v>
       </c>
@@ -7442,7 +7454,7 @@
         <v>43865</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>1022</v>
       </c>
@@ -7465,7 +7477,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>1078</v>
       </c>
@@ -7488,7 +7500,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>930</v>
       </c>
@@ -7508,6 +7520,29 @@
         <v>7</v>
       </c>
       <c r="G262" s="19">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>1093</v>
+      </c>
+      <c r="B263" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="C263" t="s">
+        <v>16</v>
+      </c>
+      <c r="D263" t="s">
+        <v>14</v>
+      </c>
+      <c r="E263" t="s">
+        <v>10</v>
+      </c>
+      <c r="F263" t="s">
+        <v>7</v>
+      </c>
+      <c r="G263" s="19">
         <v>43867</v>
       </c>
     </row>
@@ -7559,12 +7594,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -7575,7 +7610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -7586,7 +7621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -7597,7 +7632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -7608,7 +7643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -7627,92 +7662,92 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
Daily tasks solving (Contest day)
</commit_message>
<xml_diff>
--- a/Interview preposition 2019-2020.xlsx
+++ b/Interview preposition 2019-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65967647-AA44-48B8-BBCB-1FC844883AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E750D052-E62B-4983-8586-0A4A77F3FA90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5148" yWindow="708" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="303">
   <si>
     <t>Number</t>
   </si>
@@ -922,6 +922,15 @@
   </si>
   <si>
     <t>Average of Levels in Binary Tree</t>
+  </si>
+  <si>
+    <t>Number of Steps to Reduce a Number to Zero</t>
+  </si>
+  <si>
+    <t>Number of Sub-arrays of Size K and Average Greater than or Equal to Threshold</t>
+  </si>
+  <si>
+    <t>Angle Between Hands of a Clock</t>
   </si>
 </sst>
 </file>
@@ -931,12 +940,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1117,7 +1134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1126,20 +1143,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1498,16 +1516,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:G266"/>
+  <dimension ref="A1:G269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
-      <selection activeCell="B266" sqref="B266"/>
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="54.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5546875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -7631,6 +7649,75 @@
       </c>
       <c r="G266" s="19">
         <v>43868</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>1342</v>
+      </c>
+      <c r="B267" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C267" t="s">
+        <v>19</v>
+      </c>
+      <c r="D267" t="s">
+        <v>12</v>
+      </c>
+      <c r="E267" t="s">
+        <v>11</v>
+      </c>
+      <c r="F267" t="s">
+        <v>8</v>
+      </c>
+      <c r="G267" s="19">
+        <v>43869</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>1343</v>
+      </c>
+      <c r="B268" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C268" t="s">
+        <v>15</v>
+      </c>
+      <c r="D268" t="s">
+        <v>14</v>
+      </c>
+      <c r="E268" t="s">
+        <v>11</v>
+      </c>
+      <c r="F268" t="s">
+        <v>8</v>
+      </c>
+      <c r="G268" s="19">
+        <v>43869</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>1344</v>
+      </c>
+      <c r="B269" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="C269" t="s">
+        <v>16</v>
+      </c>
+      <c r="D269" t="s">
+        <v>14</v>
+      </c>
+      <c r="E269" t="s">
+        <v>11</v>
+      </c>
+      <c r="F269" t="s">
+        <v>8</v>
+      </c>
+      <c r="G269" s="19">
+        <v>43869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>